<commit_message>
Added new features and bug fixes
</commit_message>
<xml_diff>
--- a/dist/stamp_data.xlsx
+++ b/dist/stamp_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\pyextension\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53C1521-9FC5-4AF7-A67B-A7C8F6366182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F64274D-0B37-4833-9394-65A16EC2086E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Purchased_by</t>
   </si>
@@ -60,17 +60,20 @@
     <t>Consideration_Price</t>
   </si>
   <si>
-    <t>JIO FINANCE LIMITED</t>
-  </si>
-  <si>
-    <t>OTHERS</t>
+    <t>SILVER TOUCH TECHNOLOGIES LIMITED</t>
+  </si>
+  <si>
+    <t>CMS COMPUTERS INDIA PRIVATE LIMITED</t>
+  </si>
+  <si>
+    <t>AGREEMENT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +100,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -141,9 +150,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,17 +457,17 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
@@ -499,13 +506,15 @@
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+      <c r="B2" t="s">
+        <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
       <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
@@ -513,7 +522,7 @@
         <v>300</v>
       </c>
       <c r="H2" s="2">
-        <v>9891284481</v>
+        <v>9979894159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>